<commit_message>
dataset creation, modeling, agents
</commit_message>
<xml_diff>
--- a/Data/Odds/NCAAB/ncaa basketball 2021-22.xlsx
+++ b/Data/Odds/NCAAB/ncaa basketball 2021-22.xlsx
@@ -81124,10 +81124,8 @@
       <c r="J2061" t="n">
         <v>-185</v>
       </c>
-      <c r="K2061" t="inlineStr">
-        <is>
-          <t>.5ev</t>
-        </is>
+      <c r="K2061" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="2062">

</xml_diff>